<commit_message>
Update Despesas and Receitas UI components to set default selections; refactor server logic for improved data handling; adjust bundle ID in deployment configuration; replace outdated Excel data file.
</commit_message>
<xml_diff>
--- a/dados/2429 Prudencia jan-mar.xlsx
+++ b/dados/2429 Prudencia jan-mar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://incorporadoraampla.sharepoint.com/sites/Controladoria/Documentos Compartilhados/amplaGitHub/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{2F204289-99C5-4555-AA92-E86D2F477440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16794C63-C313-48FE-9A5C-E4CBA496735A}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{2F204289-99C5-4555-AA92-E86D2F477440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63A02F5C-38CC-439E-967F-EAB9CE3B576C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-7905" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C2EAA338-EC28-4369-9395-AF61BE10B4FC}"/>
+    <workbookView minimized="1" xWindow="-23895" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{C2EAA338-EC28-4369-9395-AF61BE10B4FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Janeiro" sheetId="1" r:id="rId1"/>
@@ -2411,11 +2411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7685E717-DFE0-4950-B9E8-923B5CDAFB27}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J238"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5 H5:J5 B94:D95 H94:J95 B109:D109 H109:J109 B137:D137 H137:J137 B230:D230 H230:J230"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,7 +2508,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>2</v>
       </c>
@@ -2540,7 +2539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>3</v>
       </c>
@@ -2574,7 +2573,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>4</v>
       </c>
@@ -2608,7 +2607,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>5</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>6</v>
       </c>
@@ -2676,7 +2675,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <v>7</v>
       </c>
@@ -2710,7 +2709,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
         <v>8</v>
       </c>
@@ -2744,7 +2743,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <v>9</v>
       </c>
@@ -2778,7 +2777,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <v>10</v>
       </c>
@@ -2812,7 +2811,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
         <v>11</v>
       </c>
@@ -2846,7 +2845,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>12</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <v>13</v>
       </c>
@@ -2914,7 +2913,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>14</v>
       </c>
@@ -2948,7 +2947,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>15</v>
       </c>
@@ -2982,7 +2981,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>16</v>
       </c>
@@ -3016,7 +3015,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>17</v>
       </c>
@@ -3050,7 +3049,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>18</v>
       </c>
@@ -3084,7 +3083,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>19</v>
       </c>
@@ -3118,7 +3117,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <v>20</v>
       </c>
@@ -3152,7 +3151,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
         <v>21</v>
       </c>
@@ -3186,7 +3185,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>22</v>
       </c>
@@ -3220,7 +3219,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <v>23</v>
       </c>
@@ -3254,7 +3253,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
         <v>24</v>
       </c>
@@ -3288,7 +3287,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
         <v>25</v>
       </c>
@@ -3322,7 +3321,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
         <v>26</v>
       </c>
@@ -3356,7 +3355,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <v>27</v>
       </c>
@@ -3390,7 +3389,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>28</v>
       </c>
@@ -3424,7 +3423,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>29</v>
       </c>
@@ -3458,7 +3457,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>30</v>
       </c>
@@ -3492,7 +3491,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="15">
         <v>31</v>
       </c>
@@ -3526,7 +3525,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>32</v>
       </c>
@@ -3560,7 +3559,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <v>33</v>
       </c>
@@ -3594,7 +3593,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <v>34</v>
       </c>
@@ -3628,7 +3627,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <v>35</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15">
         <v>36</v>
       </c>
@@ -3696,7 +3695,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15">
         <v>37</v>
       </c>
@@ -3730,7 +3729,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15">
         <v>38</v>
       </c>
@@ -3764,7 +3763,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15">
         <v>39</v>
       </c>
@@ -3798,7 +3797,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>40</v>
       </c>
@@ -3832,7 +3831,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
         <v>41</v>
       </c>
@@ -3866,7 +3865,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15">
         <v>42</v>
       </c>
@@ -3900,7 +3899,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15">
         <v>43</v>
       </c>
@@ -3934,7 +3933,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="15">
         <v>44</v>
       </c>
@@ -3968,7 +3967,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="15">
         <v>45</v>
       </c>
@@ -4002,7 +4001,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="15">
         <v>46</v>
       </c>
@@ -4036,7 +4035,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15">
         <v>47</v>
       </c>
@@ -4070,7 +4069,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15">
         <v>48</v>
       </c>
@@ -4104,7 +4103,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15">
         <v>49</v>
       </c>
@@ -4138,7 +4137,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="15">
         <v>50</v>
       </c>
@@ -4172,7 +4171,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15">
         <v>51</v>
       </c>
@@ -4206,7 +4205,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="15">
         <v>52</v>
       </c>
@@ -4240,7 +4239,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="15">
         <v>53</v>
       </c>
@@ -4274,7 +4273,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="15">
         <v>54</v>
       </c>
@@ -4308,7 +4307,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="15">
         <v>55</v>
       </c>
@@ -4342,7 +4341,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15">
         <v>56</v>
       </c>
@@ -4376,7 +4375,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="15">
         <v>57</v>
       </c>
@@ -4410,7 +4409,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>58</v>
       </c>
@@ -4444,7 +4443,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
         <v>59</v>
       </c>
@@ -4478,7 +4477,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="15">
         <v>60</v>
       </c>
@@ -4512,7 +4511,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>61</v>
       </c>
@@ -4546,7 +4545,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="15">
         <v>62</v>
       </c>
@@ -4580,7 +4579,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="15">
         <v>63</v>
       </c>
@@ -4614,7 +4613,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15">
         <v>64</v>
       </c>
@@ -4648,7 +4647,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15">
         <v>65</v>
       </c>
@@ -4682,7 +4681,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="15">
         <v>66</v>
       </c>
@@ -4716,7 +4715,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="15">
         <v>67</v>
       </c>
@@ -4750,7 +4749,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="15">
         <v>68</v>
       </c>
@@ -4784,7 +4783,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="15">
         <v>69</v>
       </c>
@@ -4818,7 +4817,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="15">
         <v>70</v>
       </c>
@@ -4852,7 +4851,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="15">
         <v>71</v>
       </c>
@@ -4886,7 +4885,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="15">
         <v>72</v>
       </c>
@@ -4920,7 +4919,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="15">
         <v>73</v>
       </c>
@@ -4954,7 +4953,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="15">
         <v>74</v>
       </c>
@@ -4988,7 +4987,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15">
         <v>75</v>
       </c>
@@ -5022,7 +5021,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="15">
         <v>76</v>
       </c>
@@ -5056,7 +5055,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="15">
         <v>77</v>
       </c>
@@ -5090,7 +5089,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="15">
         <v>78</v>
       </c>
@@ -5124,7 +5123,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="15">
         <v>79</v>
       </c>
@@ -5158,7 +5157,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="15">
         <v>80</v>
       </c>
@@ -5192,7 +5191,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="15">
         <v>81</v>
       </c>
@@ -5226,7 +5225,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="15">
         <v>82</v>
       </c>
@@ -5257,7 +5256,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="15">
         <v>83</v>
       </c>
@@ -5291,7 +5290,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="15">
         <v>84</v>
       </c>
@@ -5325,7 +5324,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="15">
         <v>85</v>
       </c>
@@ -5359,7 +5358,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="15">
         <v>86</v>
       </c>
@@ -5393,7 +5392,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="15">
         <v>87</v>
       </c>
@@ -5424,7 +5423,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="15">
         <v>88</v>
       </c>
@@ -5455,7 +5454,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="15">
         <v>89</v>
       </c>
@@ -5554,7 +5553,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="15">
         <v>92</v>
       </c>
@@ -5585,7 +5584,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="15">
         <v>93</v>
       </c>
@@ -5616,7 +5615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="15">
         <v>94</v>
       </c>
@@ -5647,7 +5646,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="15">
         <v>95</v>
       </c>
@@ -5678,7 +5677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="15">
         <v>96</v>
       </c>
@@ -5709,7 +5708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="15">
         <v>97</v>
       </c>
@@ -5740,7 +5739,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="15">
         <v>98</v>
       </c>
@@ -5771,7 +5770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="15">
         <v>99</v>
       </c>
@@ -5802,7 +5801,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="15">
         <v>100</v>
       </c>
@@ -5833,7 +5832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="15">
         <v>101</v>
       </c>
@@ -5864,7 +5863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="15">
         <v>102</v>
       </c>
@@ -5895,7 +5894,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="15">
         <v>103</v>
       </c>
@@ -5926,7 +5925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="15">
         <v>104</v>
       </c>
@@ -5991,7 +5990,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="15">
         <v>106</v>
       </c>
@@ -6022,7 +6021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="15">
         <v>107</v>
       </c>
@@ -6053,7 +6052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="15">
         <v>108</v>
       </c>
@@ -6084,7 +6083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="15">
         <v>109</v>
       </c>
@@ -6115,7 +6114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="15">
         <v>110</v>
       </c>
@@ -6146,7 +6145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="15">
         <v>111</v>
       </c>
@@ -6177,7 +6176,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="15">
         <v>112</v>
       </c>
@@ -6208,7 +6207,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="15">
         <v>113</v>
       </c>
@@ -6239,7 +6238,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="15">
         <v>114</v>
       </c>
@@ -6270,7 +6269,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="15">
         <v>115</v>
       </c>
@@ -6301,7 +6300,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="15">
         <v>116</v>
       </c>
@@ -6332,7 +6331,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="15">
         <v>117</v>
       </c>
@@ -6363,7 +6362,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="15">
         <v>118</v>
       </c>
@@ -6394,7 +6393,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="15">
         <v>119</v>
       </c>
@@ -6425,7 +6424,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="15">
         <v>120</v>
       </c>
@@ -6456,7 +6455,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="15">
         <v>121</v>
       </c>
@@ -6487,7 +6486,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="15">
         <v>122</v>
       </c>
@@ -6518,7 +6517,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="15">
         <v>123</v>
       </c>
@@ -6549,7 +6548,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="15">
         <v>124</v>
       </c>
@@ -6580,7 +6579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="15">
         <v>125</v>
       </c>
@@ -6611,7 +6610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="15">
         <v>126</v>
       </c>
@@ -6642,7 +6641,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="15">
         <v>127</v>
       </c>
@@ -6673,7 +6672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="15">
         <v>128</v>
       </c>
@@ -6704,7 +6703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="15">
         <v>129</v>
       </c>
@@ -6735,7 +6734,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="15">
         <v>130</v>
       </c>
@@ -6766,7 +6765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="15">
         <v>131</v>
       </c>
@@ -6797,7 +6796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="15">
         <v>132</v>
       </c>
@@ -6862,7 +6861,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="15">
         <v>134</v>
       </c>
@@ -6893,7 +6892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="15">
         <v>135</v>
       </c>
@@ -6924,7 +6923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="15">
         <v>136</v>
       </c>
@@ -6955,7 +6954,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="15">
         <v>137</v>
       </c>
@@ -6986,7 +6985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="15">
         <v>138</v>
       </c>
@@ -7017,7 +7016,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="15">
         <v>139</v>
       </c>
@@ -7048,7 +7047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="15">
         <v>140</v>
       </c>
@@ -7082,7 +7081,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="15">
         <v>141</v>
       </c>
@@ -7116,7 +7115,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="15">
         <v>142</v>
       </c>
@@ -7150,7 +7149,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="15">
         <v>143</v>
       </c>
@@ -7184,7 +7183,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="15">
         <v>144</v>
       </c>
@@ -7218,7 +7217,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="15">
         <v>145</v>
       </c>
@@ -7252,7 +7251,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="15">
         <v>146</v>
       </c>
@@ -7286,7 +7285,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="15">
         <v>147</v>
       </c>
@@ -7320,7 +7319,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="15">
         <v>148</v>
       </c>
@@ -7354,7 +7353,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="15">
         <v>149</v>
       </c>
@@ -7388,7 +7387,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="15">
         <v>150</v>
       </c>
@@ -7422,7 +7421,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="15">
         <v>151</v>
       </c>
@@ -7456,7 +7455,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="15">
         <v>152</v>
       </c>
@@ -7490,7 +7489,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="15">
         <v>153</v>
       </c>
@@ -7524,7 +7523,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="15">
         <v>154</v>
       </c>
@@ -7558,7 +7557,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="15">
         <v>155</v>
       </c>
@@ -7592,7 +7591,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="15">
         <v>156</v>
       </c>
@@ -7626,7 +7625,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="15">
         <v>157</v>
       </c>
@@ -7660,7 +7659,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="15">
         <v>158</v>
       </c>
@@ -7694,7 +7693,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="15">
         <v>159</v>
       </c>
@@ -7728,7 +7727,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="15">
         <v>160</v>
       </c>
@@ -7762,7 +7761,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="165" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="15">
         <v>161</v>
       </c>
@@ -7796,7 +7795,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="15">
         <v>162</v>
       </c>
@@ -7830,7 +7829,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="15">
         <v>163</v>
       </c>
@@ -7864,7 +7863,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="15">
         <v>164</v>
       </c>
@@ -7898,7 +7897,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="15">
         <v>165</v>
       </c>
@@ -7932,7 +7931,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="170" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="15">
         <v>166</v>
       </c>
@@ -7966,7 +7965,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="15">
         <v>167</v>
       </c>
@@ -8000,7 +7999,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="15">
         <v>168</v>
       </c>
@@ -8034,7 +8033,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="15">
         <v>169</v>
       </c>
@@ -8068,7 +8067,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="15">
         <v>170</v>
       </c>
@@ -8102,7 +8101,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="15">
         <v>171</v>
       </c>
@@ -8136,7 +8135,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="15">
         <v>172</v>
       </c>
@@ -8170,7 +8169,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="15">
         <v>173</v>
       </c>
@@ -8204,7 +8203,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="15">
         <v>174</v>
       </c>
@@ -8238,7 +8237,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="15">
         <v>175</v>
       </c>
@@ -8272,7 +8271,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="15">
         <v>176</v>
       </c>
@@ -8306,7 +8305,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="15">
         <v>177</v>
       </c>
@@ -8340,7 +8339,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="15">
         <v>178</v>
       </c>
@@ -8374,7 +8373,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="15">
         <v>179</v>
       </c>
@@ -8408,7 +8407,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="15">
         <v>180</v>
       </c>
@@ -8442,7 +8441,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="15">
         <v>181</v>
       </c>
@@ -8476,7 +8475,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="15">
         <v>182</v>
       </c>
@@ -8510,7 +8509,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="15">
         <v>183</v>
       </c>
@@ -8544,7 +8543,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="15">
         <v>184</v>
       </c>
@@ -8578,7 +8577,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="15">
         <v>185</v>
       </c>
@@ -8612,7 +8611,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="15">
         <v>186</v>
       </c>
@@ -8646,7 +8645,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="15">
         <v>187</v>
       </c>
@@ -8680,7 +8679,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="15">
         <v>188</v>
       </c>
@@ -8714,7 +8713,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="15">
         <v>189</v>
       </c>
@@ -8748,7 +8747,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="194" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="15">
         <v>190</v>
       </c>
@@ -8782,7 +8781,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="15">
         <v>191</v>
       </c>
@@ -8816,7 +8815,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="15">
         <v>192</v>
       </c>
@@ -8850,7 +8849,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="197" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="15">
         <v>193</v>
       </c>
@@ -8884,7 +8883,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="15">
         <v>194</v>
       </c>
@@ -8918,7 +8917,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="199" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="15">
         <v>195</v>
       </c>
@@ -8952,7 +8951,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="15">
         <v>196</v>
       </c>
@@ -8986,7 +8985,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="201" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="15">
         <v>197</v>
       </c>
@@ -9020,7 +9019,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="15">
         <v>198</v>
       </c>
@@ -9054,7 +9053,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="203" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="15">
         <v>199</v>
       </c>
@@ -9088,7 +9087,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="15">
         <v>200</v>
       </c>
@@ -9122,7 +9121,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="15">
         <v>201</v>
       </c>
@@ -9156,7 +9155,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="206" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="15">
         <v>202</v>
       </c>
@@ -9190,7 +9189,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="15">
         <v>203</v>
       </c>
@@ -9224,7 +9223,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="208" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="15">
         <v>204</v>
       </c>
@@ -9258,7 +9257,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="209" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="15">
         <v>205</v>
       </c>
@@ -9292,7 +9291,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="210" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="15">
         <v>206</v>
       </c>
@@ -9326,7 +9325,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="211" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="15">
         <v>207</v>
       </c>
@@ -9360,7 +9359,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="212" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="15">
         <v>208</v>
       </c>
@@ -9394,7 +9393,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="213" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="15">
         <v>209</v>
       </c>
@@ -9428,7 +9427,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="214" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="15">
         <v>210</v>
       </c>
@@ -9462,7 +9461,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="215" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="15">
         <v>211</v>
       </c>
@@ -9496,7 +9495,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="216" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="15">
         <v>212</v>
       </c>
@@ -9530,7 +9529,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="217" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="15">
         <v>213</v>
       </c>
@@ -9564,7 +9563,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="218" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="15">
         <v>214</v>
       </c>
@@ -9598,7 +9597,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="219" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="15">
         <v>215</v>
       </c>
@@ -9632,7 +9631,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="220" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="15">
         <v>216</v>
       </c>
@@ -9666,7 +9665,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="221" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="15">
         <v>217</v>
       </c>
@@ -9700,7 +9699,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="222" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="15">
         <v>218</v>
       </c>
@@ -9734,7 +9733,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="223" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="15">
         <v>219</v>
       </c>
@@ -9768,7 +9767,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="224" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="15">
         <v>220</v>
       </c>
@@ -9802,7 +9801,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="225" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="15">
         <v>221</v>
       </c>
@@ -9836,7 +9835,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="226" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="15">
         <v>222</v>
       </c>
@@ -9870,7 +9869,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="227" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="15">
         <v>223</v>
       </c>
@@ -9904,7 +9903,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="228" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="15">
         <v>224</v>
       </c>
@@ -9935,7 +9934,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="229" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="15">
         <v>225</v>
       </c>
@@ -10000,7 +9999,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="231" spans="1:10" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="15">
         <v>227</v>
       </c>
@@ -10072,16 +10071,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J231" xr:uid="{7685E717-DFE0-4950-B9E8-923B5CDAFB27}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="debito fiador juros de obra - pf"/>
-        <filter val="Parcela PJ"/>
-        <filter val="pgto de saldo pj"/>
-        <filter val="tarifa caixa medição"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A4:J231" xr:uid="{7685E717-DFE0-4950-B9E8-923B5CDAFB27}"/>
   <mergeCells count="1">
     <mergeCell ref="B3:I3"/>
   </mergeCells>
@@ -10110,7 +10100,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D11 H10:J11 B18:D18 H18:J18 B27:D27 H27:J27"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11151,8 +11141,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98:D100 H98:J100 B104:D104 H104:J104 B120:D120 H120:J120"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="63.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15079,26 +15069,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5a5f483f-f768-438e-b4ef-63f46a7558dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="dd8c73df-45bd-468c-aae5-f3faedcbd5e2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006C56FB2846673243A9735D5EC6051572" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="941ba21155b641a9d77936be19967558">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5a5f483f-f768-438e-b4ef-63f46a7558dd" xmlns:ns3="dd8c73df-45bd-468c-aae5-f3faedcbd5e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="469d177505629adaca6589b93d36bf5c" ns2:_="" ns3:_="">
     <xsd:import namespace="5a5f483f-f768-438e-b4ef-63f46a7558dd"/>
@@ -15293,26 +15263,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0825223-2C7D-4797-A314-F6957DB6A27A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5a5f483f-f768-438e-b4ef-63f46a7558dd"/>
-    <ds:schemaRef ds:uri="dd8c73df-45bd-468c-aae5-f3faedcbd5e2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1246CCEC-0DEC-4D6F-A217-935ADD40F756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5a5f483f-f768-438e-b4ef-63f46a7558dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="dd8c73df-45bd-468c-aae5-f3faedcbd5e2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3F8109-51B1-4692-864E-6B54FF554F65}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15329,4 +15300,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1246CCEC-0DEC-4D6F-A217-935ADD40F756}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0825223-2C7D-4797-A314-F6957DB6A27A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a5f483f-f768-438e-b4ef-63f46a7558dd"/>
+    <ds:schemaRef ds:uri="dd8c73df-45bd-468c-aae5-f3faedcbd5e2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>